<commit_message>
aggiornato report-checklist.xlsx come richiesto
aggiornato report-checklist.xlsx come richiesto
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#CGMTELEMEDICINESRLXX/CGM_Telemedicine_Srl/CGMCAREMAP/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#CGMTELEMEDICINESRLXX/CGM_Telemedicine_Srl/CGMCAREMAP/4.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgm01-my.sharepoint.com/personal/denis_nani_cgm_com/Documents/Documentazione/HP/CDA e FSE/accreditamento/Test Case/A1#111#CGMTELEMEDICINESRLXX/CGM_Telemedicine_Srl/CGMCAREMAP/4.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="290" documentId="8_{B47AD472-6D29-47A2-98E3-B20B04674961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{815B0017-0C86-45BA-8BAB-CCA285B98EAD}"/>
+  <xr:revisionPtr revIDLastSave="301" documentId="8_{B47AD472-6D29-47A2-98E3-B20B04674961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F698FC5-74AF-4E19-BB56-343637323551}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="187">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -706,9 +706,6 @@
   </si>
   <si>
     <t>CGM Telemedicine s.r.l.</t>
-  </si>
-  <si>
-    <t>Non vengono gestite le sezioni opzionali</t>
   </si>
   <si>
     <t>ATTENZIONE: il codice fiscale dell'assistito non è stato inserito correttamente. Si prega di corregere i dati il prima possibile</t>
@@ -2892,10 +2889,10 @@
   <dimension ref="A1:W592"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="M10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomRight" activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3199,13 +3196,13 @@
         <v>42</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H10" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I10" s="39"/>
       <c r="J10" s="35" t="s">
@@ -3220,15 +3217,19 @@
         <v>49</v>
       </c>
       <c r="O10" s="35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P10" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="35"/>
+      <c r="Q10" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="R10" s="35" t="s">
+        <v>76</v>
+      </c>
       <c r="S10" s="35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T10" s="35"/>
       <c r="U10" s="36"/>
@@ -3254,13 +3255,13 @@
         <v>47</v>
       </c>
       <c r="F11" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="H11" s="34" t="s">
         <v>186</v>
-      </c>
-      <c r="G11" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>187</v>
       </c>
       <c r="I11" s="39"/>
       <c r="J11" s="35" t="s">
@@ -3275,15 +3276,19 @@
         <v>49</v>
       </c>
       <c r="O11" s="35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P11" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
+      <c r="Q11" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="R11" s="35" t="s">
+        <v>76</v>
+      </c>
       <c r="S11" s="35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T11" s="35"/>
       <c r="U11" s="36"/>
@@ -3324,7 +3329,7 @@
         <v>49</v>
       </c>
       <c r="O12" s="35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P12" s="35" t="s">
         <v>76</v>
@@ -3336,7 +3341,7 @@
         <v>76</v>
       </c>
       <c r="S12" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T12" s="35"/>
       <c r="U12" s="36" t="s">
@@ -3364,16 +3369,16 @@
         <v>107</v>
       </c>
       <c r="F13" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="H13" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="G13" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="H13" s="34" t="s">
+      <c r="I13" s="39" t="s">
         <v>158</v>
-      </c>
-      <c r="I13" s="39" t="s">
-        <v>159</v>
       </c>
       <c r="J13" s="35" t="s">
         <v>49</v>
@@ -3387,7 +3392,7 @@
         <v>49</v>
       </c>
       <c r="O13" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="P13" s="35" t="s">
         <v>76</v>
@@ -3399,7 +3404,7 @@
         <v>76</v>
       </c>
       <c r="S13" s="35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T13" s="35"/>
       <c r="U13" s="36"/>
@@ -3425,16 +3430,16 @@
         <v>108</v>
       </c>
       <c r="F14" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="H14" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="G14" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="H14" s="34" t="s">
+      <c r="I14" s="39" t="s">
         <v>161</v>
-      </c>
-      <c r="I14" s="39" t="s">
-        <v>162</v>
       </c>
       <c r="J14" s="35" t="s">
         <v>49</v>
@@ -3448,7 +3453,7 @@
         <v>49</v>
       </c>
       <c r="O14" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P14" s="35" t="s">
         <v>76</v>
@@ -3460,7 +3465,7 @@
         <v>76</v>
       </c>
       <c r="S14" s="35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T14" s="35"/>
       <c r="U14" s="36"/>
@@ -3568,16 +3573,16 @@
         <v>56</v>
       </c>
       <c r="F17" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="H17" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="G17" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="H17" s="34" t="s">
+      <c r="I17" s="39" t="s">
         <v>164</v>
-      </c>
-      <c r="I17" s="39" t="s">
-        <v>165</v>
       </c>
       <c r="J17" s="35" t="s">
         <v>49</v>
@@ -3591,7 +3596,7 @@
         <v>49</v>
       </c>
       <c r="O17" s="35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P17" s="35" t="s">
         <v>76</v>
@@ -3603,7 +3608,7 @@
         <v>76</v>
       </c>
       <c r="S17" s="35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T17" s="35"/>
       <c r="U17" s="36"/>
@@ -3629,16 +3634,16 @@
         <v>58</v>
       </c>
       <c r="F18" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="H18" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="G18" s="34" t="s">
-        <v>166</v>
-      </c>
-      <c r="H18" s="34" t="s">
+      <c r="I18" s="39" t="s">
         <v>167</v>
-      </c>
-      <c r="I18" s="39" t="s">
-        <v>168</v>
       </c>
       <c r="J18" s="35" t="s">
         <v>49</v>
@@ -3652,7 +3657,7 @@
         <v>49</v>
       </c>
       <c r="O18" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P18" s="35" t="s">
         <v>76</v>
@@ -3664,7 +3669,7 @@
         <v>76</v>
       </c>
       <c r="S18" s="35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T18" s="35"/>
       <c r="U18" s="36"/>
@@ -3690,16 +3695,16 @@
         <v>98</v>
       </c>
       <c r="F19" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="H19" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="G19" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="H19" s="34" t="s">
+      <c r="I19" s="39" t="s">
         <v>170</v>
-      </c>
-      <c r="I19" s="39" t="s">
-        <v>171</v>
       </c>
       <c r="J19" s="35" t="s">
         <v>49</v>
@@ -3713,7 +3718,7 @@
         <v>49</v>
       </c>
       <c r="O19" s="35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P19" s="35" t="s">
         <v>76</v>
@@ -3725,7 +3730,7 @@
         <v>76</v>
       </c>
       <c r="S19" s="35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T19" s="35"/>
       <c r="U19" s="36"/>
@@ -3760,9 +3765,7 @@
       <c r="K20" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="L20" s="35" t="s">
-        <v>144</v>
-      </c>
+      <c r="L20" s="35"/>
       <c r="M20" s="35"/>
       <c r="N20" s="35"/>
       <c r="O20" s="35"/>
@@ -3794,16 +3797,16 @@
         <v>100</v>
       </c>
       <c r="F21" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="H21" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="G21" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="H21" s="34" t="s">
+      <c r="I21" s="39" t="s">
         <v>173</v>
-      </c>
-      <c r="I21" s="39" t="s">
-        <v>174</v>
       </c>
       <c r="J21" s="35" t="s">
         <v>49</v>
@@ -3817,7 +3820,7 @@
         <v>49</v>
       </c>
       <c r="O21" s="35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P21" s="35" t="s">
         <v>76</v>
@@ -3829,7 +3832,7 @@
         <v>76</v>
       </c>
       <c r="S21" s="35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T21" s="35"/>
       <c r="U21" s="36"/>
@@ -3864,9 +3867,7 @@
       <c r="K22" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="L22" s="35" t="s">
-        <v>144</v>
-      </c>
+      <c r="L22" s="35"/>
       <c r="M22" s="35"/>
       <c r="N22" s="35"/>
       <c r="O22" s="35"/>
@@ -3907,9 +3908,7 @@
       <c r="K23" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="L23" s="35" t="s">
-        <v>144</v>
-      </c>
+      <c r="L23" s="35"/>
       <c r="M23" s="35"/>
       <c r="N23" s="35"/>
       <c r="O23" s="35"/>
@@ -3950,9 +3949,7 @@
       <c r="K24" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="L24" s="35" t="s">
-        <v>144</v>
-      </c>
+      <c r="L24" s="35"/>
       <c r="M24" s="35"/>
       <c r="N24" s="35"/>
       <c r="O24" s="35"/>
@@ -3993,9 +3990,7 @@
       <c r="K25" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="L25" s="35" t="s">
-        <v>144</v>
-      </c>
+      <c r="L25" s="35"/>
       <c r="M25" s="35"/>
       <c r="N25" s="35"/>
       <c r="O25" s="35"/>
@@ -4036,9 +4031,7 @@
       <c r="K26" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="L26" s="35" t="s">
-        <v>144</v>
-      </c>
+      <c r="L26" s="35"/>
       <c r="M26" s="35"/>
       <c r="N26" s="35"/>
       <c r="O26" s="35"/>
@@ -4111,16 +4104,16 @@
         <v>118</v>
       </c>
       <c r="F28" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="G28" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="H28" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="G28" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="H28" s="34" t="s">
+      <c r="I28" s="39" t="s">
         <v>176</v>
-      </c>
-      <c r="I28" s="39" t="s">
-        <v>177</v>
       </c>
       <c r="J28" s="35" t="s">
         <v>49</v>
@@ -4158,16 +4151,16 @@
         <v>119</v>
       </c>
       <c r="F29" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="G29" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="H29" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="G29" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="H29" s="34" t="s">
+      <c r="I29" s="39" t="s">
         <v>179</v>
-      </c>
-      <c r="I29" s="39" t="s">
-        <v>180</v>
       </c>
       <c r="J29" s="35" t="s">
         <v>49</v>
@@ -4214,9 +4207,7 @@
       <c r="K30" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="L30" s="35" t="s">
-        <v>144</v>
-      </c>
+      <c r="L30" s="35"/>
       <c r="M30" s="35"/>
       <c r="N30" s="35"/>
       <c r="O30" s="33"/>
@@ -4289,16 +4280,16 @@
         <v>136</v>
       </c>
       <c r="F32" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="H32" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="G32" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="H32" s="34" t="s">
+      <c r="I32" s="39" t="s">
         <v>182</v>
-      </c>
-      <c r="I32" s="39" t="s">
-        <v>183</v>
       </c>
       <c r="J32" s="35" t="s">
         <v>49</v>
@@ -4312,7 +4303,7 @@
         <v>49</v>
       </c>
       <c r="O32" s="35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P32" s="35" t="s">
         <v>76</v>
@@ -4324,7 +4315,7 @@
         <v>76</v>
       </c>
       <c r="S32" s="35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T32" s="35"/>
       <c r="U32" s="36"/>
@@ -10646,12 +10637,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10913,21 +10907,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10952,18 +10952,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
aggiornati test 448 e 449
aggiornati test 448 e 449
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#CGMTELEMEDICINESRLXX/CGM_Telemedicine_Srl/CGMCAREMAP/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#CGMTELEMEDICINESRLXX/CGM_Telemedicine_Srl/CGMCAREMAP/4.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgm01-my.sharepoint.com/personal/denis_nani_cgm_com/Documents/Documentazione/HP/CDA e FSE/accreditamento/Test Case/A1#111#CGMTELEMEDICINESRLXX/CGM_Telemedicine_Srl/CGMCAREMAP/4.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="309" documentId="8_{B47AD472-6D29-47A2-98E3-B20B04674961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFE7E341-24B1-4743-8EE3-DFE8CAB3A04A}"/>
+  <xr:revisionPtr revIDLastSave="317" documentId="8_{B47AD472-6D29-47A2-98E3-B20B04674961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3B34DDD-A2CE-4E27-AC31-EE8C91493D8E}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -819,22 +819,22 @@
     <t>369b984ac430e6e0a2114b886d639cd1</t>
   </si>
   <si>
-    <t>2025-07-07T10:02:45Z</t>
-  </si>
-  <si>
-    <t>da16db0c2196f5a056de034117ecefc3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.54eb38f4c2faa7993d6e20b2357a4c4312889bde043689cb1e6a131820ca8a04.31bed564aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-07-07T10:05:00Z</t>
-  </si>
-  <si>
-    <t>9947ad6131608320f6f5f7bd9b6db447</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.54eb38f4c2faa7993d6e20b2357a4c4312889bde043689cb1e6a131820ca8a04.a77ccab4e4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-07-09T17:43:23Z</t>
+  </si>
+  <si>
+    <t>4c68c9a47563b60047b120232b8a161f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.54eb38f4c2faa7993d6e20b2357a4c4312889bde043689cb1e6a131820ca8a04.2959431b4d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-07-09T17:42:06Z</t>
+  </si>
+  <si>
+    <t>1a8d230c2b5f82ae970d6520b09b8c58</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.54eb38f4c2faa7993d6e20b2357a4c4312889bde043689cb1e6a131820ca8a04.dd2c0792fa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4104,16 +4104,16 @@
         <v>118</v>
       </c>
       <c r="F28" s="34" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H28" s="34" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="I28" s="39" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="J28" s="35" t="s">
         <v>49</v>
@@ -4151,16 +4151,16 @@
         <v>119</v>
       </c>
       <c r="F29" s="34" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G29" s="34" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H29" s="34" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I29" s="39" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="J29" s="35" t="s">
         <v>49</v>
@@ -10637,12 +10637,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10904,21 +10907,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10943,18 +10952,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>